<commit_message>
sample code to read from workbook
</commit_message>
<xml_diff>
--- a/sampleinput/m1.xlsx
+++ b/sampleinput/m1.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="tasksheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -104,6 +104,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -199,12 +200,12 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.2"/>
   </cols>

</xml_diff>